<commit_message>
se borran archivos innecesarios y se deja la combinacion de palbras por linea tematica y no por colores
</commit_message>
<xml_diff>
--- a/src/listado.xlsx
+++ b/src/listado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4bc5085ef5d50236/Escritorio/webScrappingFunding/WebScraping_Finding/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sague\Desktop\WebScrapping\WebScraping_Finding\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FAEF54-DF3B-4038-B98D-642D450F91DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3D1BE2-17EC-4C69-9147-4F44D3091D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -529,7 +529,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +542,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,17 +584,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -889,16 +900,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,7 +941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -949,11 +966,11 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -982,7 +999,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1011,7 +1028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1040,7 +1057,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1069,7 +1086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1098,7 +1115,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1127,7 +1144,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1156,7 +1173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1185,7 +1202,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1214,7 +1231,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1243,7 +1260,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1272,7 +1289,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1301,7 +1318,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1330,7 +1347,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1359,7 +1376,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1388,7 +1405,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1417,7 +1434,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1446,7 +1463,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1475,7 +1492,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1504,7 +1521,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1533,7 +1550,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1562,7 +1579,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1591,7 +1608,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1620,7 +1637,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1649,7 +1666,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1678,7 +1695,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1707,7 +1724,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1736,7 +1753,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1765,7 +1782,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1794,7 +1811,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1823,7 +1840,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1852,7 +1869,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1881,7 +1898,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1910,7 +1927,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1939,7 +1956,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1968,7 +1985,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1998,6 +2015,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{9A8F7CF5-4B02-4F74-A0F8-E88210246E44}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>